<commit_message>
implemented spatial branch and bound
</commit_message>
<xml_diff>
--- a/examples/PoolingContract/results.xlsx
+++ b/examples/PoolingContract/results.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33780" windowHeight="19540" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33780" windowHeight="19540" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="rootnode" sheetId="1" r:id="rId1"/>
+    <sheet name="branchAndBound" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="34">
   <si>
     <t>Cross Decomposition</t>
   </si>
@@ -38,21 +39,9 @@
     <t>-----------------</t>
   </si>
   <si>
-    <t>Iteration Value : -1338.2355348924657</t>
-  </si>
-  <si>
-    <t>Iteration Bound : -1354.2667698798525</t>
-  </si>
-  <si>
-    <t>Objective Value : -1338.2355348924657</t>
-  </si>
-  <si>
     <t>Best Bound : -1354.2667698798525</t>
   </si>
   <si>
-    <t>Gap : 1.18 %</t>
-  </si>
-  <si>
     <t>Iteration Time : 1.07 s</t>
   </si>
   <si>
@@ -108,6 +97,36 @@
   </si>
   <si>
     <t>Elapsed Time : 119.47 s</t>
+  </si>
+  <si>
+    <t>LB</t>
+  </si>
+  <si>
+    <t>UB</t>
+  </si>
+  <si>
+    <t>active nodes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gap </t>
+  </si>
+  <si>
+    <t>Number of nodes</t>
+  </si>
+  <si>
+    <t>Iteration Value : -1335.7347667524655</t>
+  </si>
+  <si>
+    <t>Iteration Bound : -1354.2667698798532</t>
+  </si>
+  <si>
+    <t>Objective Value : -1335.736749892465</t>
+  </si>
+  <si>
+    <t>Benders time</t>
+  </si>
+  <si>
+    <t>Lagrangean time</t>
   </si>
 </sst>
 </file>
@@ -150,9 +169,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -432,8 +452,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L33" sqref="L33"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -448,7 +468,7 @@
         <v>0</v>
       </c>
       <c r="D1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="F1" t="s">
         <v>1</v>
@@ -464,7 +484,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D3" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="F3" t="s">
         <v>3</v>
@@ -475,68 +495,68 @@
         <v>3</v>
       </c>
       <c r="F4" t="s">
-        <v>4</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D5" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="F5" t="s">
-        <v>5</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D6" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="F6" t="s">
-        <v>6</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D7" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="F7" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D8" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="F8" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D9" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="F9" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D10" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="F10" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D11" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D14" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
@@ -546,7 +566,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="D16" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -556,37 +576,37 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D18" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D19" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D20" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D21" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D22" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D23" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D24" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
@@ -599,7 +619,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D27" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
@@ -609,37 +629,156 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D29" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D30" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D31" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D32" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="33" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D33" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="34" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D34" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="35" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D35" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" t="s">
         <v>27</v>
+      </c>
+      <c r="F1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E2" s="2"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>21</v>
+      </c>
+      <c r="B3">
+        <v>-1355.1</v>
+      </c>
+      <c r="C3">
+        <v>-1338.88</v>
+      </c>
+      <c r="D3">
+        <v>4</v>
+      </c>
+      <c r="E3" s="2">
+        <f>-(C3-B3)/B3</f>
+        <v>1.1969596339753377E-2</v>
+      </c>
+      <c r="F3">
+        <v>674</v>
+      </c>
+      <c r="G3">
+        <v>1160</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>101</v>
+      </c>
+      <c r="B4">
+        <v>-1343.34</v>
+      </c>
+      <c r="C4">
+        <v>-1338.88</v>
+      </c>
+      <c r="D4">
+        <v>11</v>
+      </c>
+      <c r="E4" s="2">
+        <f>-(C4-B4)/B4</f>
+        <v>3.3200827787453731E-3</v>
+      </c>
+      <c r="F4">
+        <v>1368</v>
+      </c>
+      <c r="G4">
+        <v>4121</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>501</v>
+      </c>
+      <c r="B5">
+        <v>-1340.32</v>
+      </c>
+      <c r="C5">
+        <v>-1338.88</v>
+      </c>
+      <c r="D5">
+        <v>48</v>
+      </c>
+      <c r="E5" s="2">
+        <f>-(C5-B5)/B5</f>
+        <v>1.0743702996298102E-3</v>
+      </c>
+      <c r="F5">
+        <v>7631</v>
+      </c>
+      <c r="G5">
+        <v>11455</v>
       </c>
     </row>
   </sheetData>

</xml_diff>